<commit_message>
update the reactor type
</commit_message>
<xml_diff>
--- a/_input/reactor_data_raw.xlsx
+++ b/_input/reactor_data_raw.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0c3325f57cbbe622/SKOLEARBEID/Master/MasterOPPGAVE/julialange kode til masteroppgave/_input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="406" documentId="8_{7696E0A4-7455-4CF4-88F8-3006FA44D15C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{702E7CF0-644C-46C1-8DB3-35044DF09BA5}"/>
+  <xr:revisionPtr revIDLastSave="410" documentId="8_{7696E0A4-7455-4CF4-88F8-3006FA44D15C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3CDB361C-5F0B-42B5-B2EE-50F5FC43E1E0}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{7180C01F-BAB0-43C4-8B6A-D12813804A36}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="13900" xr2:uid="{7180C01F-BAB0-43C4-8B6A-D12813804A36}"/>
   </bookViews>
   <sheets>
     <sheet name="Datasheet" sheetId="1" r:id="rId1"/>
@@ -35,6 +35,28 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -775,7 +797,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
@@ -808,9 +830,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -1456,43 +1475,43 @@
   <dimension ref="B1:V163"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="X11" sqref="X11"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.26953125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="3.140625" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.5703125" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" customWidth="1"/>
+    <col min="1" max="1" width="3.1796875" customWidth="1"/>
+    <col min="2" max="2" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.54296875" customWidth="1"/>
+    <col min="4" max="4" width="16.453125" customWidth="1"/>
     <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.7109375" customWidth="1"/>
-    <col min="7" max="7" width="21.7109375" customWidth="1"/>
-    <col min="8" max="8" width="27.5703125" customWidth="1"/>
-    <col min="9" max="9" width="30.28515625" customWidth="1"/>
+    <col min="6" max="6" width="27.7265625" customWidth="1"/>
+    <col min="7" max="7" width="21.7265625" customWidth="1"/>
+    <col min="8" max="8" width="27.54296875" customWidth="1"/>
+    <col min="9" max="9" width="30.26953125" customWidth="1"/>
     <col min="10" max="10" width="38" customWidth="1"/>
-    <col min="11" max="11" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="20.28515625" customWidth="1"/>
-    <col min="16" max="16" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="34.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.1796875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.1796875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.453125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20.26953125" customWidth="1"/>
+    <col min="16" max="16" width="21.1796875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="34.453125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>4</v>
       </c>
@@ -1554,7 +1573,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="4" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>45</v>
       </c>
@@ -1617,7 +1636,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="5" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>54</v>
       </c>
@@ -1680,7 +1699,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="6" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>45</v>
       </c>
@@ -1743,7 +1762,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="7" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>159</v>
       </c>
@@ -1806,7 +1825,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="8" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>45</v>
       </c>
@@ -1869,7 +1888,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="9" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>92</v>
       </c>
@@ -1932,7 +1951,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="10" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>93</v>
       </c>
@@ -1995,7 +2014,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="11" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>92</v>
       </c>
@@ -2058,7 +2077,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="12" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
         <v>160</v>
       </c>
@@ -2118,7 +2137,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="13" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
         <v>161</v>
       </c>
@@ -2179,7 +2198,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="14" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
         <v>93</v>
       </c>
@@ -2243,7 +2262,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="15" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
         <v>201</v>
       </c>
@@ -2251,12 +2270,12 @@
         <v>22</v>
       </c>
       <c r="D15" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E15" t="s">
         <v>129</v>
       </c>
-      <c r="F15" s="22" t="str">
+      <c r="F15" s="12" t="str">
         <f>IF(Table2[[#This Row],[Capacity (net MWe)]]&lt;=50,"Micro",IF(Table2[[#This Row],[Capacity (net MWe)]]&lt;=500,"SMR","Large"))</f>
         <v>SMR</v>
       </c>
@@ -2276,7 +2295,7 @@
       <c r="M15">
         <v>90</v>
       </c>
-      <c r="O15" s="23">
+      <c r="O15" s="22">
         <v>136630</v>
       </c>
       <c r="P15" s="15">
@@ -2298,7 +2317,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="16" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
         <v>91</v>
       </c>
@@ -2358,7 +2377,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="17" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
         <v>93</v>
       </c>
@@ -2421,7 +2440,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="18" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
         <v>162</v>
       </c>
@@ -2481,7 +2500,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="19" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
         <v>91</v>
       </c>
@@ -2541,7 +2560,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="20" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
         <v>91</v>
       </c>
@@ -2549,7 +2568,7 @@
         <v>27</v>
       </c>
       <c r="D20" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E20" t="s">
         <v>133</v>
@@ -2601,7 +2620,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="21" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B21" t="s">
         <v>45</v>
       </c>
@@ -2661,7 +2680,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="22" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
         <v>92</v>
       </c>
@@ -2721,7 +2740,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="23" spans="2:21" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:21" ht="29" x14ac:dyDescent="0.35">
       <c r="B23" s="12" t="s">
         <v>45</v>
       </c>
@@ -2782,7 +2801,7 @@
         <v>1987</v>
       </c>
     </row>
-    <row r="24" spans="2:21" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:21" ht="29" x14ac:dyDescent="0.35">
       <c r="B24" s="12" t="s">
         <v>45</v>
       </c>
@@ -2843,7 +2862,7 @@
         <v>1986</v>
       </c>
     </row>
-    <row r="25" spans="2:21" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:21" ht="29" x14ac:dyDescent="0.35">
       <c r="B25" s="12" t="s">
         <v>45</v>
       </c>
@@ -2904,7 +2923,7 @@
         <v>1985</v>
       </c>
     </row>
-    <row r="26" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B26" s="12" t="s">
         <v>163</v>
       </c>
@@ -2965,7 +2984,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="27" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B27" s="12" t="s">
         <v>163</v>
       </c>
@@ -3026,7 +3045,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="28" spans="2:21" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B28" s="12" t="s">
         <v>164</v>
       </c>
@@ -3087,7 +3106,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="29" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B29" s="12" t="s">
         <v>164</v>
       </c>
@@ -3148,7 +3167,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="30" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B30" s="12" t="s">
         <v>54</v>
       </c>
@@ -3207,7 +3226,7 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="31" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B31" s="12" t="s">
         <v>54</v>
       </c>
@@ -3266,7 +3285,7 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="32" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:21" x14ac:dyDescent="0.35">
       <c r="B32" s="12" t="s">
         <v>45</v>
       </c>
@@ -3327,7 +3346,7 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="33" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:22" x14ac:dyDescent="0.35">
       <c r="B33" s="12" t="s">
         <v>45</v>
       </c>
@@ -3388,7 +3407,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="34" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:22" x14ac:dyDescent="0.35">
       <c r="B34" s="12" t="s">
         <v>45</v>
       </c>
@@ -3449,7 +3468,7 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="35" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:22" x14ac:dyDescent="0.35">
       <c r="B35" s="12" t="s">
         <v>45</v>
       </c>
@@ -3510,7 +3529,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="36" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:22" x14ac:dyDescent="0.35">
       <c r="B36" s="12" t="s">
         <v>159</v>
       </c>
@@ -3571,7 +3590,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="37" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:22" x14ac:dyDescent="0.35">
       <c r="B37" s="12" t="s">
         <v>159</v>
       </c>
@@ -3632,7 +3651,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="38" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:22" x14ac:dyDescent="0.35">
       <c r="B38" s="12" t="s">
         <v>93</v>
       </c>
@@ -3696,7 +3715,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="39" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:22" x14ac:dyDescent="0.35">
       <c r="B39" s="12" t="s">
         <v>93</v>
       </c>
@@ -3760,7 +3779,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="40" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:22" x14ac:dyDescent="0.35">
       <c r="B40" s="12" t="s">
         <v>93</v>
       </c>
@@ -3821,7 +3840,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="41" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:22" x14ac:dyDescent="0.35">
       <c r="B41" s="12" t="s">
         <v>93</v>
       </c>
@@ -3882,7 +3901,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="42" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:22" x14ac:dyDescent="0.35">
       <c r="B42" s="12" t="s">
         <v>92</v>
       </c>
@@ -3943,7 +3962,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="43" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:22" x14ac:dyDescent="0.35">
       <c r="B43" s="12" t="s">
         <v>92</v>
       </c>
@@ -4004,7 +4023,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="44" spans="2:22" ht="30" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:22" x14ac:dyDescent="0.35">
       <c r="B44" s="12" t="s">
         <v>45</v>
       </c>
@@ -4065,7 +4084,7 @@
         <v>1976</v>
       </c>
     </row>
-    <row r="45" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:22" x14ac:dyDescent="0.35">
       <c r="B45" s="12" t="s">
         <v>45</v>
       </c>
@@ -4126,7 +4145,7 @@
         <v>1976</v>
       </c>
     </row>
-    <row r="46" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:22" x14ac:dyDescent="0.35">
       <c r="B46" s="12" t="s">
         <v>45</v>
       </c>
@@ -4187,7 +4206,7 @@
         <v>1967</v>
       </c>
     </row>
-    <row r="47" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:22" x14ac:dyDescent="0.35">
       <c r="B47" s="12" t="s">
         <v>92</v>
       </c>
@@ -4250,7 +4269,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="48" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:22" x14ac:dyDescent="0.35">
       <c r="B48" s="12" t="s">
         <v>164</v>
       </c>
@@ -4311,7 +4330,7 @@
         <v>1986</v>
       </c>
     </row>
-    <row r="49" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B49" t="s">
         <v>92</v>
       </c>
@@ -4335,7 +4354,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="50" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B50" t="s">
         <v>92</v>
       </c>
@@ -4359,7 +4378,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="51" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B51" t="s">
         <v>159</v>
       </c>
@@ -4383,7 +4402,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="52" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B52" t="s">
         <v>159</v>
       </c>
@@ -4407,27 +4426,73 @@
         <v>11</v>
       </c>
     </row>
-    <row r="53" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:11" x14ac:dyDescent="0.35">
       <c r="F53" s="12"/>
       <c r="J53" s="16"/>
       <c r="K53" s="12"/>
     </row>
-    <row r="54" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:11" x14ac:dyDescent="0.35">
       <c r="F54" s="12"/>
       <c r="J54" s="16"/>
       <c r="K54" s="12"/>
     </row>
-    <row r="71" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="D56" t="str" cm="1">
+        <f t="array" ref="D56:D64">_xlfn.UNIQUE(D4:D52)</f>
+        <v>BWR</v>
+      </c>
+    </row>
+    <row r="57" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="D57" t="str">
+        <v>PWR</v>
+      </c>
+    </row>
+    <row r="58" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="D58" t="str">
+        <v>HTR</v>
+      </c>
+    </row>
+    <row r="59" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="D59" t="str">
+        <v>HTGR</v>
+      </c>
+    </row>
+    <row r="60" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="D60" t="str">
+        <v>SFR</v>
+      </c>
+    </row>
+    <row r="61" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="D61" t="str">
+        <v>MSR</v>
+      </c>
+    </row>
+    <row r="62" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="D62" t="str">
+        <v>MSFR</v>
+      </c>
+    </row>
+    <row r="63" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="D63" t="str">
+        <v>MR</v>
+      </c>
+    </row>
+    <row r="64" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="D64" t="str">
+        <v>LFR</v>
+      </c>
+    </row>
+    <row r="71" spans="2:9" x14ac:dyDescent="0.35">
       <c r="I71" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="72" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:9" x14ac:dyDescent="0.35">
       <c r="I72" s="6" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="73" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:9" x14ac:dyDescent="0.35">
       <c r="D73" s="1" t="s">
         <v>42</v>
       </c>
@@ -4438,7 +4503,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="74" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B74" s="7" t="s">
         <v>4</v>
       </c>
@@ -4464,7 +4529,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="75" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B75" t="s">
         <v>12</v>
       </c>
@@ -4488,7 +4553,7 @@
         <v>2587500</v>
       </c>
     </row>
-    <row r="76" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B76" t="s">
         <v>54</v>
       </c>
@@ -4512,7 +4577,7 @@
         <v>6363914.1049661394</v>
       </c>
     </row>
-    <row r="77" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B77" t="s">
         <v>45</v>
       </c>
@@ -4536,7 +4601,7 @@
         <v>7259374.9999999991</v>
       </c>
     </row>
-    <row r="78" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B78" t="s">
         <v>86</v>
       </c>
@@ -4560,7 +4625,7 @@
         <v>10948554.579439251</v>
       </c>
     </row>
-    <row r="79" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B79" t="s">
         <v>45</v>
       </c>
@@ -4584,7 +4649,7 @@
         <v>3985899.9999999995</v>
       </c>
     </row>
-    <row r="80" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B80" t="s">
         <v>70</v>
       </c>
@@ -4608,7 +4673,7 @@
         <v>4403454.5454545449</v>
       </c>
     </row>
-    <row r="81" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B81" t="s">
         <v>85</v>
       </c>
@@ -4632,7 +4697,7 @@
         <v>12264749.999999998</v>
       </c>
     </row>
-    <row r="82" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B82" t="s">
         <v>70</v>
       </c>
@@ -4656,7 +4721,7 @@
         <v>17020000.5390625</v>
       </c>
     </row>
-    <row r="83" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B83" t="s">
         <v>87</v>
       </c>
@@ -4680,7 +4745,7 @@
         <v>30932124.999999996</v>
       </c>
     </row>
-    <row r="84" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B84" t="s">
         <v>45</v>
       </c>
@@ -4704,7 +4769,7 @@
         <v>5408864.4339622641</v>
       </c>
     </row>
-    <row r="85" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B85" t="s">
         <v>85</v>
       </c>
@@ -4728,7 +4793,7 @@
         <v>6520499.9999999991</v>
       </c>
     </row>
-    <row r="86" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B86" t="s">
         <v>89</v>
       </c>
@@ -4752,7 +4817,7 @@
         <v>2160606.0606060605</v>
       </c>
     </row>
-    <row r="87" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B87" t="s">
         <v>90</v>
       </c>
@@ -4776,7 +4841,7 @@
         <v>5807500</v>
       </c>
     </row>
-    <row r="88" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B88" t="s">
         <v>93</v>
       </c>
@@ -4800,7 +4865,7 @@
         <v>26489716.399999999</v>
       </c>
     </row>
-    <row r="89" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B89" t="s">
         <v>88</v>
       </c>
@@ -4824,7 +4889,7 @@
         <v>2875000</v>
       </c>
     </row>
-    <row r="90" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B90" t="s">
         <v>91</v>
       </c>
@@ -4848,7 +4913,7 @@
         <v>4662405.8999999994</v>
       </c>
     </row>
-    <row r="91" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B91" t="s">
         <v>54</v>
       </c>
@@ -4872,7 +4937,7 @@
         <v>2242500</v>
       </c>
     </row>
-    <row r="92" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B92" t="s">
         <v>45</v>
       </c>
@@ -4896,7 +4961,7 @@
         <v>6637143.3499999996</v>
       </c>
     </row>
-    <row r="93" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B93" t="s">
         <v>92</v>
       </c>
@@ -4920,13 +4985,13 @@
         <v>4784000</v>
       </c>
     </row>
-    <row r="96" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:8" x14ac:dyDescent="0.35">
       <c r="D96" t="s">
         <v>30</v>
       </c>
       <c r="G96" s="3"/>
     </row>
-    <row r="98" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="98" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C98" t="s">
         <v>4</v>
       </c>
@@ -4949,7 +5014,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="99" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="99" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C99" t="s">
         <v>45</v>
       </c>
@@ -4969,7 +5034,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="100" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="100" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C100" t="s">
         <v>45</v>
       </c>
@@ -4989,7 +5054,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="101" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="101" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C101" t="s">
         <v>45</v>
       </c>
@@ -5009,7 +5074,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="102" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="102" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C102" t="s">
         <v>49</v>
       </c>
@@ -5029,7 +5094,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="103" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C103" t="s">
         <v>49</v>
       </c>
@@ -5049,7 +5114,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="104" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="104" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C104" t="s">
         <v>52</v>
       </c>
@@ -5069,7 +5134,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="105" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C105" t="s">
         <v>52</v>
       </c>
@@ -5089,7 +5154,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="106" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="106" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C106" t="s">
         <v>54</v>
       </c>
@@ -5106,7 +5171,7 @@
         <v>8549</v>
       </c>
     </row>
-    <row r="107" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="107" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C107" t="s">
         <v>54</v>
       </c>
@@ -5126,7 +5191,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="108" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="108" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C108" t="s">
         <v>45</v>
       </c>
@@ -5146,7 +5211,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="109" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C109" t="s">
         <v>45</v>
       </c>
@@ -5166,7 +5231,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="110" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C110" t="s">
         <v>45</v>
       </c>
@@ -5186,7 +5251,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="111" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="111" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C111" t="s">
         <v>45</v>
       </c>
@@ -5206,7 +5271,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="112" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="112" spans="3:9" x14ac:dyDescent="0.35">
       <c r="C112" t="s">
         <v>61</v>
       </c>
@@ -5223,7 +5288,7 @@
         <v>2410</v>
       </c>
     </row>
-    <row r="113" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="113" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C113" t="s">
         <v>61</v>
       </c>
@@ -5240,7 +5305,7 @@
         <v>2410</v>
       </c>
     </row>
-    <row r="114" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="114" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C114" t="s">
         <v>65</v>
       </c>
@@ -5257,7 +5322,7 @@
         <v>3154</v>
       </c>
     </row>
-    <row r="115" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="115" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C115" t="s">
         <v>65</v>
       </c>
@@ -5274,7 +5339,7 @@
         <v>3154</v>
       </c>
     </row>
-    <row r="116" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="116" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C116" t="s">
         <v>65</v>
       </c>
@@ -5291,7 +5356,7 @@
         <v>3222</v>
       </c>
     </row>
-    <row r="117" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="117" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C117" t="s">
         <v>65</v>
       </c>
@@ -5308,7 +5373,7 @@
         <v>3222</v>
       </c>
     </row>
-    <row r="118" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="118" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C118" t="s">
         <v>70</v>
       </c>
@@ -5325,7 +5390,7 @@
         <v>2244</v>
       </c>
     </row>
-    <row r="119" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="119" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C119" t="s">
         <v>70</v>
       </c>
@@ -5342,7 +5407,7 @@
         <v>2244</v>
       </c>
     </row>
-    <row r="120" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="120" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C120" t="s">
         <v>45</v>
       </c>
@@ -5362,7 +5427,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="121" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="121" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C121" t="s">
         <v>45</v>
       </c>
@@ -5382,7 +5447,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="122" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C122" t="s">
         <v>45</v>
       </c>
@@ -5399,7 +5464,7 @@
         <v>1197</v>
       </c>
     </row>
-    <row r="123" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="123" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C123" t="s">
         <v>70</v>
       </c>
@@ -5416,7 +5481,7 @@
         <v>2501</v>
       </c>
     </row>
-    <row r="124" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="124" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C124" t="s">
         <v>52</v>
       </c>
@@ -5433,12 +5498,12 @@
         <v>27747</v>
       </c>
     </row>
-    <row r="141" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="141" spans="6:7" x14ac:dyDescent="0.35">
       <c r="G141" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="142" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="142" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F142">
         <v>2250</v>
       </c>
@@ -5447,7 +5512,7 @@
         <v>2250000</v>
       </c>
     </row>
-    <row r="143" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="143" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F143">
         <v>5215.9369999999999</v>
       </c>
@@ -5456,7 +5521,7 @@
         <v>5215937</v>
       </c>
     </row>
-    <row r="144" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="144" spans="6:7" x14ac:dyDescent="0.35">
       <c r="F144">
         <v>6312.5</v>
       </c>
@@ -5465,7 +5530,7 @@
         <v>6312500</v>
       </c>
     </row>
-    <row r="145" spans="6:14" x14ac:dyDescent="0.25">
+    <row r="145" spans="6:14" x14ac:dyDescent="0.35">
       <c r="F145">
         <v>8000</v>
       </c>
@@ -5474,7 +5539,7 @@
         <v>8000000</v>
       </c>
     </row>
-    <row r="146" spans="6:14" x14ac:dyDescent="0.25">
+    <row r="146" spans="6:14" x14ac:dyDescent="0.35">
       <c r="F146">
         <v>3600</v>
       </c>
@@ -5483,7 +5548,7 @@
         <v>3600000</v>
       </c>
     </row>
-    <row r="147" spans="6:14" x14ac:dyDescent="0.25">
+    <row r="147" spans="6:14" x14ac:dyDescent="0.35">
       <c r="F147">
         <v>4212</v>
       </c>
@@ -5492,7 +5557,7 @@
         <v>4212000</v>
       </c>
     </row>
-    <row r="148" spans="6:14" x14ac:dyDescent="0.25">
+    <row r="148" spans="6:14" x14ac:dyDescent="0.35">
       <c r="F148">
         <v>8532</v>
       </c>
@@ -5501,7 +5566,7 @@
         <v>8532000</v>
       </c>
     </row>
-    <row r="149" spans="6:14" x14ac:dyDescent="0.25">
+    <row r="149" spans="6:14" x14ac:dyDescent="0.35">
       <c r="F149">
         <v>13531.429</v>
       </c>
@@ -5510,7 +5575,7 @@
         <v>13531429</v>
       </c>
     </row>
-    <row r="150" spans="6:14" x14ac:dyDescent="0.25">
+    <row r="150" spans="6:14" x14ac:dyDescent="0.35">
       <c r="F150">
         <v>23187.5</v>
       </c>
@@ -5519,7 +5584,7 @@
         <v>23187500</v>
       </c>
     </row>
-    <row r="151" spans="6:14" x14ac:dyDescent="0.25">
+    <row r="151" spans="6:14" x14ac:dyDescent="0.35">
       <c r="F151">
         <v>4373.3</v>
       </c>
@@ -5528,7 +5593,7 @@
         <v>4373300</v>
       </c>
     </row>
-    <row r="152" spans="6:14" x14ac:dyDescent="0.25">
+    <row r="152" spans="6:14" x14ac:dyDescent="0.35">
       <c r="F152">
         <v>3270</v>
       </c>
@@ -5552,7 +5617,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="153" spans="6:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="153" spans="6:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="F153">
         <v>5050</v>
       </c>
@@ -5577,7 +5642,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="154" spans="6:14" ht="60" x14ac:dyDescent="0.25">
+    <row r="154" spans="6:14" ht="58" x14ac:dyDescent="0.35">
       <c r="F154">
         <v>19350</v>
       </c>
@@ -5600,7 +5665,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="155" spans="6:14" ht="60" x14ac:dyDescent="0.25">
+    <row r="155" spans="6:14" ht="58" x14ac:dyDescent="0.35">
       <c r="F155">
         <v>6900</v>
       </c>
@@ -5623,7 +5688,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="156" spans="6:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="156" spans="6:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="F156">
         <v>4054.2660000000001</v>
       </c>
@@ -5648,7 +5713,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="157" spans="6:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="157" spans="6:14" ht="29" x14ac:dyDescent="0.35">
       <c r="F157">
         <v>1950</v>
       </c>
@@ -5671,7 +5736,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="158" spans="6:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="158" spans="6:14" ht="29" x14ac:dyDescent="0.35">
       <c r="F158">
         <v>5771.4290000000001</v>
       </c>
@@ -5694,7 +5759,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="159" spans="6:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="159" spans="6:14" ht="29" x14ac:dyDescent="0.35">
       <c r="F159">
         <v>4160</v>
       </c>
@@ -5717,7 +5782,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="160" spans="6:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="160" spans="6:14" ht="29" x14ac:dyDescent="0.35">
       <c r="J160" s="12"/>
       <c r="K160" s="12" t="s">
         <v>192</v>
@@ -5733,7 +5798,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="161" spans="10:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="161" spans="10:14" ht="29" x14ac:dyDescent="0.35">
       <c r="J161" s="12"/>
       <c r="K161" s="12" t="s">
         <v>194</v>
@@ -5749,7 +5814,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="162" spans="10:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="162" spans="10:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="J162" s="20" t="s">
         <v>196</v>
       </c>
@@ -5767,7 +5832,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="163" spans="10:14" ht="60" x14ac:dyDescent="0.25">
+    <row r="163" spans="10:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="J163" s="12"/>
       <c r="K163" s="12" t="s">
         <v>199</v>
@@ -5809,13 +5874,13 @@
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="34.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="12.5703125" customWidth="1"/>
+    <col min="2" max="2" width="34.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>2</v>
       </c>
@@ -5823,7 +5888,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>111</v>
       </c>
@@ -5834,7 +5899,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>114</v>
       </c>
@@ -5845,7 +5910,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>115</v>
       </c>
@@ -5859,7 +5924,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>116</v>
       </c>
@@ -5873,7 +5938,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>117</v>
       </c>
@@ -5884,7 +5949,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>127</v>
       </c>
@@ -5905,14 +5970,14 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="2.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>140</v>
       </c>
@@ -5926,17 +5991,17 @@
         <v>143</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3">
         <f ca="1">RAND()*(0.15-0.04)+0.04</f>
-        <v>7.8797321939715309E-2</v>
+        <v>0.14781379942445699</v>
       </c>
       <c r="C3">
         <f ca="1">IF(RAND()&lt;(0.9-0.75)/(0.95-0.75),0.75+SQRT(RAND()*(0.9-0.75)*(0.95-0.75)),0.95-SQRT((1-RAND())*(0.95-0.9)*(0.95-0.75)))</f>
-        <v>0.87249022256407505</v>
+        <v>0.90973758868530497</v>
       </c>
     </row>
   </sheetData>
@@ -5945,11 +6010,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="e404e11a-1b7c-46a4-be41-f958fe29f57e" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6162,27 +6228,17 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="e404e11a-1b7c-46a4-be41-f958fe29f57e" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AF9096D1-AE55-4C5A-977F-80A54D8830AA}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D7E6B785-65A1-4A39-A7DA-3AAC95355A33}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="e404e11a-1b7c-46a4-be41-f958fe29f57e"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="022a34b1-9d82-4dd2-8ef7-65dd835f832c"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -6207,9 +6263,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D7E6B785-65A1-4A39-A7DA-3AAC95355A33}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AF9096D1-AE55-4C5A-977F-80A54D8830AA}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="e404e11a-1b7c-46a4-be41-f958fe29f57e"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="022a34b1-9d82-4dd2-8ef7-65dd835f832c"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>